<commit_message>
In Progress - WorkOrder Loading
</commit_message>
<xml_diff>
--- a/Loading/WorkOrders/CurrentCycle/Data/WorkOrders - Template.xlsx
+++ b/Loading/WorkOrders/CurrentCycle/Data/WorkOrders - Template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarathonConsultant\Documents\GitHub\AssetWorksConversion\Loading\WorkOrders\CurrentCycle\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="123">
   <si>
     <t>Job status</t>
   </si>
@@ -86,54 +91,9 @@
     <t>2037</t>
   </si>
   <si>
-    <t>188:2</t>
-  </si>
-  <si>
-    <t>188:3</t>
-  </si>
-  <si>
-    <t>188:4</t>
-  </si>
-  <si>
-    <t>189:2</t>
-  </si>
-  <si>
-    <t>189:6</t>
-  </si>
-  <si>
-    <t>189:9</t>
-  </si>
-  <si>
-    <t>189:11</t>
-  </si>
-  <si>
-    <t>189:18</t>
-  </si>
-  <si>
-    <t>189:31</t>
-  </si>
-  <si>
-    <t>189:45</t>
-  </si>
-  <si>
-    <t>189:62</t>
-  </si>
-  <si>
-    <t>189:65</t>
-  </si>
-  <si>
-    <t>189:15</t>
-  </si>
-  <si>
-    <t>189:34</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
-    <t>189:36</t>
-  </si>
-  <si>
     <t>Task ID</t>
   </si>
   <si>
@@ -143,9 +103,6 @@
     <t>Tasks</t>
   </si>
   <si>
-    <t>[GROUPROW]</t>
-  </si>
-  <si>
     <t>Work Accomplished Code (WAC)</t>
   </si>
   <si>
@@ -302,36 +259,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>188:8</t>
-  </si>
-  <si>
-    <t>189:38</t>
-  </si>
-  <si>
-    <t>189:40</t>
-  </si>
-  <si>
-    <t>189:42</t>
-  </si>
-  <si>
-    <t>189:47</t>
-  </si>
-  <si>
-    <t>189:50</t>
-  </si>
-  <si>
-    <t>189:61</t>
-  </si>
-  <si>
-    <t>189:64</t>
-  </si>
-  <si>
-    <t>189:80</t>
-  </si>
-  <si>
-    <t>189:81</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -422,9 +349,6 @@
     <t>PM Service</t>
   </si>
   <si>
-    <t>189:25</t>
-  </si>
-  <si>
     <t>Decimal (5,2)</t>
   </si>
   <si>
@@ -437,19 +361,7 @@
     <t>Correction</t>
   </si>
   <si>
-    <t>8065:2</t>
-  </si>
-  <si>
-    <t>8065:4</t>
-  </si>
-  <si>
-    <t>8065:6</t>
-  </si>
-  <si>
     <t>PM Scheduled</t>
-  </si>
-  <si>
-    <t>189:27</t>
   </si>
   <si>
     <t>Update PM Schedule</t>
@@ -1311,7 +1223,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1321,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,7 +1292,7 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -1395,49 +1307,49 @@
         <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>9</v>
@@ -1449,133 +1361,63 @@
         <v>13</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="AG1" s="5" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="AH1" s="5" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="AI1" s="5" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:35" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1606,30 +1448,30 @@
         <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E2" s="1" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1637,25 +1479,25 @@
         <v>2037</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1666,22 +1508,22 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1714,42 +1556,42 @@
         <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E2" s="1" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1757,31 +1599,31 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1792,19 +1634,19 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>17</v>
@@ -1813,7 +1655,7 @@
         <v>2</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1824,28 +1666,28 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="I5" s="3">
         <v>3</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1856,28 +1698,28 @@
         <v>20</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="I6" s="3">
         <v>4</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1913,54 +1755,54 @@
         <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="E2" s="7" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1968,37 +1810,37 @@
         <v>2437</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2009,34 +1851,34 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2072,54 +1914,54 @@
         <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2127,37 +1969,37 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2168,31 +2010,31 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
In Progress - WorkOrders Loading
</commit_message>
<xml_diff>
--- a/Loading/WorkOrders/CurrentCycle/Data/WorkOrders - Template.xlsx
+++ b/Loading/WorkOrders/CurrentCycle/Data/WorkOrders - Template.xlsx
@@ -888,7 +888,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -903,7 +903,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1231,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AI1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,43 +1381,6 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1779,29 +1741,29 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="E2" s="7" t="s">
+    <row r="2" spans="1:12" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="E2" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to W/O Loading to include Standard Jobs
</commit_message>
<xml_diff>
--- a/Loading/WorkOrders/CurrentCycle/Data/WorkOrders - Template.xlsx
+++ b/Loading/WorkOrders/CurrentCycle/Data/WorkOrders - Template.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarathonConsultant\Documents\GitHub\AssetWorksConversion\Loading\WorkOrders\CurrentCycle\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -198,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,12 +334,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -696,25 +685,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1033,7 +1016,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1069,9 +1052,9 @@
     <col min="18" max="18" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="20.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -1086,109 +1069,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AG1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AI1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1200,7 +1183,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1219,50 +1202,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1271,7 +1234,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1293,72 +1256,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1367,7 +1294,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1390,70 +1317,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1462,7 +1361,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1485,56 +1384,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1558,19 +1443,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>